<commit_message>
Got the barplots working with midas taxonomy
</commit_message>
<xml_diff>
--- a/Data_summary.xlsx
+++ b/Data_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Github/Fiber-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F951674-D6AB-AF4B-A6CD-1DBB59C5D4CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C163E33D-6DFD-624D-83E9-BD5C9734984B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="1020" windowWidth="28240" windowHeight="19860" xr2:uid="{EA2D919D-7FAA-224F-8C58-70C4EEFAE19D}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16840" xr2:uid="{EA2D919D-7FAA-224F-8C58-70C4EEFAE19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet4!$A$1:$J$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="336">
   <si>
     <t>WF_40</t>
   </si>
@@ -1497,7 +1497,7 @@
   <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="O112" sqref="O112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4388,6 +4388,9 @@
       <c r="I102" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J102" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
@@ -4417,6 +4420,9 @@
       <c r="I103" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J103" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
@@ -4446,6 +4452,9 @@
       <c r="I104" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J104" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="105" spans="1:11" s="17" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
@@ -4475,7 +4484,9 @@
       <c r="I105" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="J105" s="23"/>
+      <c r="J105" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="K105" s="23"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
@@ -4506,6 +4517,9 @@
       <c r="I106" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J106" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
@@ -4535,6 +4549,9 @@
       <c r="I107" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J107" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -4564,6 +4581,9 @@
       <c r="I108" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J108" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="109" spans="1:11" s="17" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
@@ -4593,7 +4613,9 @@
       <c r="I109" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="J109" s="23"/>
+      <c r="J109" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="K109" s="23"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
@@ -4618,6 +4640,9 @@
       <c r="G110" s="2">
         <v>0</v>
       </c>
+      <c r="J110" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -4647,6 +4672,9 @@
       <c r="I111" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J111" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
@@ -4676,6 +4704,9 @@
       <c r="I112" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J112" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="113" spans="1:11" s="17" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
@@ -4705,7 +4736,9 @@
       <c r="I113" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="J113" s="23"/>
+      <c r="J113" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="K113" s="23"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
@@ -4736,6 +4769,9 @@
       <c r="I114" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J114" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
@@ -4765,6 +4801,9 @@
       <c r="I115" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J115" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
@@ -4794,6 +4833,9 @@
       <c r="I116" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J116" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
@@ -4823,6 +4865,9 @@
       <c r="I117" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="J117" s="6" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="118" spans="1:11" s="17" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
@@ -4852,7 +4897,9 @@
       <c r="I118" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="J118" s="23"/>
+      <c r="J118" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="K118" s="23"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>